<commit_message>
envio de email para responsaveis dos respondentes
</commit_message>
<xml_diff>
--- a/public/planilhas/profile_descricao.xlsx
+++ b/public/planilhas/profile_descricao.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malvim.BSA_NET\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB729A4F-B698-47AC-A480-E8F9D5D7B19F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,12 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
-    <t xml:space="preserve">Ás</t>
+    <t>Ás</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Os Ases se dão bem com os outros. Você, Fulano, com sua maneira comedida e comportamento simples, é capaz de lidar bem com diferentes perfis comportamentais. Os Ases são atentos, pacientes e geralmente determinados a contribuir com aqueles que acreditam ser amigos.",
         "Eles formam relações íntimas com um conjunto moderadamente pequeno de participantes no meio de trabalho. Mantém padrões habituais e previstos. Mais habilidosos em áreas especializadas, os Ases planejam seu trabalho por meio de canais direcionados e exercem um desempenho muito sólido. A admiração aos outros ajuda a sustentar o nível de consistência.",
@@ -45,7 +50,7 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Detalhista</t>
+    <t>Detalhista</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -69,10 +74,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Encantador</t>
+    <t>Encantador</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "As pessoas com um Perfil Encantador buscam conscientemente transformar os pensamentos e ações dos outros. Elas tendem a controlar o seu ambiente. Elas são astutas em definir e manipular as motivações das pessoas para conduzir seu comportamento em interesse de um fim certo.",
         "As pessoas Encantadoras são cristalinas quanto aos resultados que pretendem, mas nem sempre os verbalizam imediatamente. Elas só estabelecem os resultados que intencionam após terem preparado a outra pessoa, concedendo sua amizade àqueles que visam aceitação, sua autoridade àqueles que buscam poder e sua firmeza àqueles que pretendem um ambiente previsível.",
@@ -93,10 +98,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Formador</t>
+    <t>Formador</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "As pessoas com Perfil de Formador apresentam ações diferentes no seu comportamento. Seu interesse de alcançar resultados materiais é equilibrado pelo seu grande sentido de precisão e sua hostilidade é abrandada por meio de sua sensibilidade.",
         "Apesar de agir e pensar de forma rápida, eles se limitam pelo interesse de entender todos os prováveis resultados antes de considerar uma decisão.",
@@ -117,10 +122,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Habilidoso</t>
+    <t>Habilidoso</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Os Habilidosos ressaltam a sua capacidade em áreas especializadas. Estimulados pelo interesse de ser “hábil em alguma coisa”, eles minuciosamente controlam sua própria atuação de trabalho. Ainda que o seu propósito seja ser “o especialista"" em uma área, os Habilidosos frequentemente dão a impressão de que compreendem um pouco de tudo. Esta imagem é firme quando eles verbalizam sua capacidade em diversos assuntos.",
         "Ao relacionar-se com as outras pessoas, os Habilidosos esboçam um estilo tranquilo, diplomático e simples de lidar. Este comportamento agradável muda quando é necessário ter concentração para atingir um resultado de alto padrão. Visto que valorizam a auto-disciplina, os Habilidosos consideram os outros baseado na sua capacidade de concentrar-se nas atividades. Eles têm grandes perspectivas de si mesmos e dos outros e buscam verbalizar sua frustração.",
@@ -140,10 +145,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Mediador</t>
+    <t>Mediador</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Os Mediadores são mais cuidadosos com os aspectos humanos das relações e tarefas do seu trabalho. Apresentando empatia e provendo assistência, eles são bons ouvintes e são admirados por essa disposição. Os Mediadores fazem com que as pessoas se sintam desejadas e importantes. Como os Mediadores respondem às necessidades dos outros, as pessoas não sentem temor de serem rejeitadas por eles. Os Mediadores apresentam solidariedade e estão determinados a fazer atividades para os outros.",
         "Os Mediadores apresentam uma grande capacidade para elaborar e cumprir tarefas eficazmente. Os Mediadores facilmente geram equilíbrio em um trabalho de grupo e são bons em fazer para os demais o que acham difícil de realizar para si mesmos.",
@@ -163,10 +168,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Mentor</t>
+    <t>Mentor</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Ao utilizar uma prática de que “as pessoas são importantes”, os Mentores provavelmente não se atentem às realizações das tarefas. Eles às vezes precisam de ajuda para construir e realizar com limites determinados.",
         "Os Mentores frequentemente entendem a crítica como uma afronta pessoal, mas respondem bem a elogios por tarefas completadas. Numa função de responsabilidade, os Mentores buscam ser atentos à qualidade do ambiente de trabalho e reconhecem as pessoas da equipe."
@@ -185,10 +190,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Observador</t>
+    <t>Observador</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Objetivos e minuciosos, os Observadores são “exemplos de existências” apartidárias. Normalmente comedidos, eles visam equilíbrio e constantemente um sentido independente em direção a um objetivo determinado. Os Observadores obtêm resultados em diversas coisas, não por razão da sua flexibilidade mas pela sua determinação persistente de ir até o final. Eles visam um planejamento ou propósito objetivo de onde consigam apresentar um plano ordenado e traçar suas atividades. Uma vez iniciado o plano, os Observadores lutam tenazmente para realizar seus objetivos. Às vezes uma interferência é essencial para transformar seu caminho. Por isso, eles podem ser considerados como indivíduos teimosos e opiniosos.",
         "Os Observadores se dão bem em funções técnicas desafiantes na qual consigam usar informações reais para entender os dados e tirar conclusões. Eles reagem à lógica em vez do sentimento. Quando estão vendendo ou realizando marketing para uma ideia, eles obtêm mais êxito com um produto preciso.",
@@ -208,10 +213,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Persistente</t>
+    <t>Persistente</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "As pessoas Persistentes apresentam autoconfiança, o que alguns podem compreender como arrogância. Elas buscam ativamente possibilidades para testar e desempenhar sua capacidade de alcançar resultados. As pessoas Persistentes gostam de tarefas complexas, situações competitivas, ações únicas e posições “importantes”. Elas assumem responsabilidades com um ar de auto-importância e apresentam auto-satisfação uma vez que tenham realizado.",
         "As pessoas Persistentes buscam impedir condições limitantes, tais como controles diretos, análises que gastam muito tempo e trabalho de rotina. Como são enérgicas e práticas, provavelmente possuam problema com as outras pessoas. As pessoas Persistentes se vangloriam de sua liberdade e provavelmente se tornam inquietas quando envolvidas em atividades de grupo ou trabalhos de comitê. Ainda que as pessoas Persistentes normalmente optem por trabalhar sozinhas, elas provavelmente convençam os outros a ajudar em seus esforços, especialmente ao completar ações de rotina.",
@@ -231,10 +236,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Persuasivo</t>
+    <t>Persuasivo</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Os Persuasivos atuam com pessoas, esforçando- se para serem simpáticos em benefício de seus próprios propósitos. Extrovertidos e interessados em pessoas, os Persuasivos têm a tendência de obter a consideração e a confiabilidade dos outros.",
         "Podem envolver os outros em suas ideias, trazendo as pessoas e mantendo-as como clientes e amigos. Esta capacidade é especialmente válida quando as pessoas Persuasivas vendem a si mesmas ou suas ideias para alcançar posições de poder e status.",
@@ -256,10 +261,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Pioneiro</t>
+    <t>Pioneiro</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Os Pioneiros buscam ser pessoas com muita força de vontade, procurando constantemente novas perspectivas. Como são auto-suficientes e pensadores independentes, optam por obter suas próprias respostas. Levemente livres da ação limitante do grupo, os Pioneiros podem escapar do tradicional e frequentemente produzir resultados inovadores.",
         "Apesar de frequentemente usarem uma ação forte e direta, os Pioneiros também podem sabiamente utilizar as pessoas e as oportunidades. No momento em que precisam estar com outros em condições que limitam seu individualismo, os Pioneiros normalmente se tornam rudes. Eles são perseverantes na busca das soluções que desejam e farão o que for necessário para superar desafios. Além disso, têm altas expectativas dos outros e podem ser analíticos se seus padrões não forem obtidos.",
@@ -279,10 +284,10 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Planejador Carismático</t>
+    <t>Planejador Carismático</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "Os Planejadores Carismáticos usam a criatividade para realizar os seus propósitos.",
         "Eles utilizam recursos ágeis para alcançar resultados.",
@@ -306,7 +311,7 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Pragmático</t>
+    <t>Pragmático</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -332,10 +337,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Realizador</t>
+    <t>Realizador</t>
   </si>
   <si>
-    <t xml:space="preserve">{
+    <t>{
     "description": [
         "O encorajamento dos Realizadores é na maior parte interior e flui de propósitos pessoais da sua vontade. Seu comprometimento com seus próprios propósitos impedem uma aceitação imediata dos propósitos do grupo. Os Realizadores necessitam encontrar como reunir os seus propósitos pessoais aos propósitos da sociedade. Ao preservar o domínio da sentido de suas vidas, os Realizadores apresentam um forte senso de comprometimento.",
  "Os Realizadores apresentam um alto interesse pelo seu trabalho e um esforço profundo e contínuo de realizações. Eles têm o maior respeito pelo seu trabalho e, sob pressão, provavelmente hesitem em transferir afazeres. Pelo contrário, eles mesmos exercem o trabalho para assegurar que seja feito da forma correta. À medida que delegam, eles têm uma inclinação a retomar a tarefa se ela não atender suas perspectivas. Seu lema é “Se eu obtiver resultado, eu quero passar a ter o crédito, se eu fracassar, eu assumirei a culpa”.",
@@ -355,15 +360,38 @@
     }
 }</t>
   </si>
+  <si>
+    <t>Comunicativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"{
+    "description": [
+        "Os Comunicativos têm uma rede ampla de relações. Eles frequentemente são dados, socialmente capazes e alcançam relações naturalmente. Eles dificilmente agridem os outros propositadamente.",
+        "Os Comunicativos preferem situações sociais favoráveis na qual sejam capazes de aperfeiçoar e preservar suas relações. Verbalmente hábeis, eles desenvolvem suas próprias idéias e geram entusiasmo para os projetos dos outros. Sempre tem acesso a pessoas que podem ajudá-los.",
+        "Como os Comunicativos optam por relacionamento, provavelmente encontram-se menos envolvidos na orientação dos resultados das tarefas. Buscam atividades sociais, ainda que seu trabalho precise de atenção a atividades mais isoladas. Eles obtêm resultado em reuniões, comitês e debates.",
+        "Frequentemente otimistas, os Comunicativos tendem a supervalorizar a capacidade das pessoas. Eles frequentemente chegam a pontos favoráveis sem observar todos os dados. A gestão do tempo provavelmente seja desafiadora para os Comunicativos. Ao determinar um limite de tempo para conversas e discussões, eles podem lembrar a si mesmos da necessidade de “concluir” a tarefa."
+    ],
+    "features": {
+        "emotions":"está disposto a receber os outros",
+        "purpose":"reconhecimento, renome",
+        "considers":"capacidades verbais",
+        "influence":"possibilidades, favores",
+        "values":"descontração; promoção de projetos e pessoas, incluindo a si mesmo",
+        "use":"elogios, esperança",
+        "threat":"torna-se descuidado e sensível, é desorganizado",
+        "fear":"perda da aceitação social e valor próprio",
+        "productivity":"domínio do tempo, assertividade, senso de urgência, equilíbrio emocional, realização de promessas e tarefas"
+    }
+}
+"
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -371,25 +399,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -409,7 +421,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -417,82 +429,350 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B997"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="160.7"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="160.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" ht="315" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,3064 +780,3071 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="282.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" ht="345" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="282.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="305.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="282.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B104" s="4"/>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" s="4"/>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="4"/>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="4"/>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B113" s="4"/>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B114" s="4"/>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B115" s="4"/>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="4"/>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B117" s="4"/>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B118" s="4"/>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B119" s="4"/>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B120" s="4"/>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B122" s="4"/>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B123" s="4"/>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B124" s="4"/>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B125" s="4"/>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B126" s="4"/>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B127" s="4"/>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B128" s="4"/>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B129" s="4"/>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B130" s="4"/>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="4"/>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B132" s="4"/>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B133" s="4"/>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B134" s="4"/>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B135" s="4"/>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B136" s="4"/>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B137" s="4"/>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B138" s="4"/>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B139" s="4"/>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B140" s="4"/>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B141" s="4"/>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B142" s="4"/>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="4"/>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B144" s="4"/>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B145" s="4"/>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B146" s="4"/>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B147" s="4"/>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="4"/>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="4"/>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="4"/>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="4"/>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="4"/>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="4"/>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="4"/>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="4"/>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="4"/>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="4"/>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="4"/>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="4"/>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="4"/>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B168" s="4"/>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B169" s="4"/>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B170" s="4"/>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B171" s="4"/>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B172" s="4"/>
     </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B173" s="4"/>
     </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B174" s="4"/>
     </row>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B175" s="4"/>
     </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B176" s="4"/>
     </row>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B177" s="4"/>
     </row>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B178" s="4"/>
     </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B179" s="4"/>
     </row>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B180" s="4"/>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B181" s="4"/>
     </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B182" s="4"/>
     </row>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
     </row>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B184" s="4"/>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B185" s="4"/>
     </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B186" s="4"/>
     </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B187" s="4"/>
     </row>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B188" s="4"/>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B189" s="4"/>
     </row>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B190" s="4"/>
     </row>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B191" s="4"/>
     </row>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B192" s="4"/>
     </row>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B193" s="4"/>
     </row>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B194" s="4"/>
     </row>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B195" s="4"/>
     </row>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B196" s="4"/>
     </row>
-    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B197" s="4"/>
     </row>
-    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B198" s="4"/>
     </row>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B199" s="4"/>
     </row>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B200" s="4"/>
     </row>
-    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B201" s="4"/>
     </row>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B203" s="4"/>
     </row>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B204" s="4"/>
     </row>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B205" s="4"/>
     </row>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B206" s="4"/>
     </row>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B207" s="4"/>
     </row>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B208" s="4"/>
     </row>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B209" s="4"/>
     </row>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B210" s="4"/>
     </row>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B211" s="4"/>
     </row>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B212" s="4"/>
     </row>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B213" s="4"/>
     </row>
-    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B214" s="4"/>
     </row>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B215" s="4"/>
     </row>
-    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B216" s="4"/>
     </row>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B217" s="4"/>
     </row>
-    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B218" s="4"/>
     </row>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B219" s="4"/>
     </row>
-    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B220" s="4"/>
     </row>
-    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B221" s="4"/>
     </row>
-    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B222" s="4"/>
     </row>
-    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B223" s="4"/>
     </row>
-    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B224" s="4"/>
     </row>
-    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B225" s="4"/>
     </row>
-    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B226" s="4"/>
     </row>
-    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B227" s="4"/>
     </row>
-    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B228" s="4"/>
     </row>
-    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B229" s="4"/>
     </row>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B230" s="4"/>
     </row>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B231" s="4"/>
     </row>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B232" s="4"/>
     </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B233" s="4"/>
     </row>
-    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B234" s="4"/>
     </row>
-    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B235" s="4"/>
     </row>
-    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B236" s="4"/>
     </row>
-    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B237" s="4"/>
     </row>
-    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B238" s="4"/>
     </row>
-    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B239" s="4"/>
     </row>
-    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B240" s="4"/>
     </row>
-    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B241" s="4"/>
     </row>
-    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B242" s="4"/>
     </row>
-    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B243" s="4"/>
     </row>
-    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B244" s="4"/>
     </row>
-    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B245" s="4"/>
     </row>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B246" s="4"/>
     </row>
-    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B247" s="4"/>
     </row>
-    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B248" s="4"/>
     </row>
-    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B249" s="4"/>
     </row>
-    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B250" s="4"/>
     </row>
-    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B251" s="4"/>
     </row>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B252" s="4"/>
     </row>
-    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B253" s="4"/>
     </row>
-    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B254" s="4"/>
     </row>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B255" s="4"/>
     </row>
-    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B256" s="4"/>
     </row>
-    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B257" s="4"/>
     </row>
-    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B258" s="4"/>
     </row>
-    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B259" s="4"/>
     </row>
-    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B260" s="4"/>
     </row>
-    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B261" s="4"/>
     </row>
-    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B262" s="4"/>
     </row>
-    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B263" s="4"/>
     </row>
-    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B264" s="4"/>
     </row>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B265" s="4"/>
     </row>
-    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B266" s="4"/>
     </row>
-    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B267" s="4"/>
     </row>
-    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B268" s="4"/>
     </row>
-    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B269" s="4"/>
     </row>
-    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B270" s="4"/>
     </row>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B271" s="4"/>
     </row>
-    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B272" s="4"/>
     </row>
-    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B273" s="4"/>
     </row>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B274" s="4"/>
     </row>
-    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B275" s="4"/>
     </row>
-    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B276" s="4"/>
     </row>
-    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B277" s="4"/>
     </row>
-    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B278" s="4"/>
     </row>
-    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B279" s="4"/>
     </row>
-    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B280" s="4"/>
     </row>
-    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B281" s="4"/>
     </row>
-    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B282" s="4"/>
     </row>
-    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B283" s="4"/>
     </row>
-    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B284" s="4"/>
     </row>
-    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B285" s="4"/>
     </row>
-    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B286" s="4"/>
     </row>
-    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B287" s="4"/>
     </row>
-    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B288" s="4"/>
     </row>
-    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B289" s="4"/>
     </row>
-    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B290" s="4"/>
     </row>
-    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B291" s="4"/>
     </row>
-    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B292" s="4"/>
     </row>
-    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B293" s="4"/>
     </row>
-    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B294" s="4"/>
     </row>
-    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B295" s="4"/>
     </row>
-    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B296" s="4"/>
     </row>
-    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B297" s="4"/>
     </row>
-    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B298" s="4"/>
     </row>
-    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B299" s="4"/>
     </row>
-    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B300" s="4"/>
     </row>
-    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B301" s="4"/>
     </row>
-    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B302" s="4"/>
     </row>
-    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B303" s="4"/>
     </row>
-    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B304" s="4"/>
     </row>
-    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B305" s="4"/>
     </row>
-    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B306" s="4"/>
     </row>
-    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B307" s="4"/>
     </row>
-    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B308" s="4"/>
     </row>
-    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B309" s="4"/>
     </row>
-    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B310" s="4"/>
     </row>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B311" s="4"/>
     </row>
-    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B312" s="4"/>
     </row>
-    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B313" s="4"/>
     </row>
-    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B314" s="4"/>
     </row>
-    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B315" s="4"/>
     </row>
-    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B316" s="4"/>
     </row>
-    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B317" s="4"/>
     </row>
-    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B318" s="4"/>
     </row>
-    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B319" s="4"/>
     </row>
-    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B320" s="4"/>
     </row>
-    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B321" s="4"/>
     </row>
-    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B322" s="4"/>
     </row>
-    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B323" s="4"/>
     </row>
-    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B324" s="4"/>
     </row>
-    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B325" s="4"/>
     </row>
-    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B326" s="4"/>
     </row>
-    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B327" s="4"/>
     </row>
-    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B328" s="4"/>
     </row>
-    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B329" s="4"/>
     </row>
-    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B330" s="4"/>
     </row>
-    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B331" s="4"/>
     </row>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B332" s="4"/>
     </row>
-    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B333" s="4"/>
     </row>
-    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B334" s="4"/>
     </row>
-    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B335" s="4"/>
     </row>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B336" s="4"/>
     </row>
-    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B337" s="4"/>
     </row>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B338" s="4"/>
     </row>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B339" s="4"/>
     </row>
-    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B340" s="4"/>
     </row>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B341" s="4"/>
     </row>
-    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B342" s="4"/>
     </row>
-    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B343" s="4"/>
     </row>
-    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B344" s="4"/>
     </row>
-    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B345" s="4"/>
     </row>
-    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B346" s="4"/>
     </row>
-    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B347" s="4"/>
     </row>
-    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B348" s="4"/>
     </row>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B349" s="4"/>
     </row>
-    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B350" s="4"/>
     </row>
-    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B351" s="4"/>
     </row>
-    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B352" s="4"/>
     </row>
-    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B353" s="4"/>
     </row>
-    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B354" s="4"/>
     </row>
-    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B355" s="4"/>
     </row>
-    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B356" s="4"/>
     </row>
-    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B357" s="4"/>
     </row>
-    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B358" s="4"/>
     </row>
-    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B359" s="4"/>
     </row>
-    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B360" s="4"/>
     </row>
-    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B361" s="4"/>
     </row>
-    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B362" s="4"/>
     </row>
-    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B363" s="4"/>
     </row>
-    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B364" s="4"/>
     </row>
-    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B365" s="4"/>
     </row>
-    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B366" s="4"/>
     </row>
-    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B367" s="4"/>
     </row>
-    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B368" s="4"/>
     </row>
-    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B369" s="4"/>
     </row>
-    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B370" s="4"/>
     </row>
-    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B371" s="4"/>
     </row>
-    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B372" s="4"/>
     </row>
-    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B373" s="4"/>
     </row>
-    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B374" s="4"/>
     </row>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B375" s="4"/>
     </row>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="376" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B376" s="4"/>
     </row>
-    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B377" s="4"/>
     </row>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="378" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B378" s="4"/>
     </row>
-    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="379" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B379" s="4"/>
     </row>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B380" s="4"/>
     </row>
-    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B381" s="4"/>
     </row>
-    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B382" s="4"/>
     </row>
-    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B383" s="4"/>
     </row>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B384" s="4"/>
     </row>
-    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="385" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B385" s="4"/>
     </row>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B386" s="4"/>
     </row>
-    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="387" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B387" s="4"/>
     </row>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B388" s="4"/>
     </row>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="389" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B389" s="4"/>
     </row>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B390" s="4"/>
     </row>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="391" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B391" s="4"/>
     </row>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="392" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B392" s="4"/>
     </row>
-    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="393" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B393" s="4"/>
     </row>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="394" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B394" s="4"/>
     </row>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="395" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B395" s="4"/>
     </row>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="396" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B396" s="4"/>
     </row>
-    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="397" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B397" s="4"/>
     </row>
-    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="398" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B398" s="4"/>
     </row>
-    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="399" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B399" s="4"/>
     </row>
-    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="400" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B400" s="4"/>
     </row>
-    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B401" s="4"/>
     </row>
-    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B402" s="4"/>
     </row>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B403" s="4"/>
     </row>
-    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="404" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B404" s="4"/>
     </row>
-    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="405" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B405" s="4"/>
     </row>
-    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B406" s="4"/>
     </row>
-    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="407" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B407" s="4"/>
     </row>
-    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="408" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B408" s="4"/>
     </row>
-    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B409" s="4"/>
     </row>
-    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="410" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B410" s="4"/>
     </row>
-    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="411" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B411" s="4"/>
     </row>
-    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B412" s="4"/>
     </row>
-    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="413" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B413" s="4"/>
     </row>
-    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B414" s="4"/>
     </row>
-    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B415" s="4"/>
     </row>
-    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="416" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B416" s="4"/>
     </row>
-    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B417" s="4"/>
     </row>
-    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B418" s="4"/>
     </row>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="419" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B419" s="4"/>
     </row>
-    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B420" s="4"/>
     </row>
-    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B421" s="4"/>
     </row>
-    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="422" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B422" s="4"/>
     </row>
-    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="423" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B423" s="4"/>
     </row>
-    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B424" s="4"/>
     </row>
-    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B425" s="4"/>
     </row>
-    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B426" s="4"/>
     </row>
-    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="427" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B427" s="4"/>
     </row>
-    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="428" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B428" s="4"/>
     </row>
-    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B429" s="4"/>
     </row>
-    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="430" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B430" s="4"/>
     </row>
-    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="431" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B431" s="4"/>
     </row>
-    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="432" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B432" s="4"/>
     </row>
-    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="433" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B433" s="4"/>
     </row>
-    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="434" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B434" s="4"/>
     </row>
-    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="435" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B435" s="4"/>
     </row>
-    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="436" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B436" s="4"/>
     </row>
-    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B437" s="4"/>
     </row>
-    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="438" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B438" s="4"/>
     </row>
-    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="439" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B439" s="4"/>
     </row>
-    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="440" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B440" s="4"/>
     </row>
-    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="441" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B441" s="4"/>
     </row>
-    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B442" s="4"/>
     </row>
-    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="443" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B443" s="4"/>
     </row>
-    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B444" s="4"/>
     </row>
-    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B445" s="4"/>
     </row>
-    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="446" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B446" s="4"/>
     </row>
-    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B447" s="4"/>
     </row>
-    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="448" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B448" s="4"/>
     </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="449" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B449" s="4"/>
     </row>
-    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="450" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B450" s="4"/>
     </row>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="451" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B451" s="4"/>
     </row>
-    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="452" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B452" s="4"/>
     </row>
-    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="453" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B453" s="4"/>
     </row>
-    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="454" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B454" s="4"/>
     </row>
-    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="455" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B455" s="4"/>
     </row>
-    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="456" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B456" s="4"/>
     </row>
-    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="457" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B457" s="4"/>
     </row>
-    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="458" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B458" s="4"/>
     </row>
-    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="459" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B459" s="4"/>
     </row>
-    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="460" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B460" s="4"/>
     </row>
-    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="461" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B461" s="4"/>
     </row>
-    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="462" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B462" s="4"/>
     </row>
-    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="463" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B463" s="4"/>
     </row>
-    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="464" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B464" s="4"/>
     </row>
-    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="465" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B465" s="4"/>
     </row>
-    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="466" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B466" s="4"/>
     </row>
-    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="467" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B467" s="4"/>
     </row>
-    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B468" s="4"/>
     </row>
-    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="469" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B469" s="4"/>
     </row>
-    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="470" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B470" s="4"/>
     </row>
-    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="471" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B471" s="4"/>
     </row>
-    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="472" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B472" s="4"/>
     </row>
-    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="473" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B473" s="4"/>
     </row>
-    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="474" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B474" s="4"/>
     </row>
-    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="475" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B475" s="4"/>
     </row>
-    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="476" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B476" s="4"/>
     </row>
-    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="477" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B477" s="4"/>
     </row>
-    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="478" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B478" s="4"/>
     </row>
-    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="479" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B479" s="4"/>
     </row>
-    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="480" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B480" s="4"/>
     </row>
-    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="481" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B481" s="4"/>
     </row>
-    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="482" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B482" s="4"/>
     </row>
-    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="483" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B483" s="4"/>
     </row>
-    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="484" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B484" s="4"/>
     </row>
-    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="485" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B485" s="4"/>
     </row>
-    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="486" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B486" s="4"/>
     </row>
-    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="487" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B487" s="4"/>
     </row>
-    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="488" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B488" s="4"/>
     </row>
-    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="489" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B489" s="4"/>
     </row>
-    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="490" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B490" s="4"/>
     </row>
-    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="491" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B491" s="4"/>
     </row>
-    <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="492" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B492" s="4"/>
     </row>
-    <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="493" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B493" s="4"/>
     </row>
-    <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="494" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B494" s="4"/>
     </row>
-    <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="495" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B495" s="4"/>
     </row>
-    <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="496" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B496" s="4"/>
     </row>
-    <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="497" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B497" s="4"/>
     </row>
-    <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="498" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B498" s="4"/>
     </row>
-    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="499" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B499" s="4"/>
     </row>
-    <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="500" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B500" s="4"/>
     </row>
-    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="501" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B501" s="4"/>
     </row>
-    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="502" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B502" s="4"/>
     </row>
-    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="503" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B503" s="4"/>
     </row>
-    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="504" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B504" s="4"/>
     </row>
-    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="505" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B505" s="4"/>
     </row>
-    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="506" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B506" s="4"/>
     </row>
-    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="507" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B507" s="4"/>
     </row>
-    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="508" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B508" s="4"/>
     </row>
-    <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="509" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B509" s="4"/>
     </row>
-    <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="510" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B510" s="4"/>
     </row>
-    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="511" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B511" s="4"/>
     </row>
-    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="512" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B512" s="4"/>
     </row>
-    <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="513" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B513" s="4"/>
     </row>
-    <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="514" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B514" s="4"/>
     </row>
-    <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="515" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B515" s="4"/>
     </row>
-    <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="516" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B516" s="4"/>
     </row>
-    <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="517" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B517" s="4"/>
     </row>
-    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="518" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B518" s="4"/>
     </row>
-    <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="519" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B519" s="4"/>
     </row>
-    <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="520" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B520" s="4"/>
     </row>
-    <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="521" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B521" s="4"/>
     </row>
-    <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="522" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B522" s="4"/>
     </row>
-    <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="523" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B523" s="4"/>
     </row>
-    <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="524" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B524" s="4"/>
     </row>
-    <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="525" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B525" s="4"/>
     </row>
-    <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="526" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B526" s="4"/>
     </row>
-    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="527" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B527" s="4"/>
     </row>
-    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="528" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B528" s="4"/>
     </row>
-    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="529" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B529" s="4"/>
     </row>
-    <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="530" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B530" s="4"/>
     </row>
-    <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="531" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B531" s="4"/>
     </row>
-    <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="532" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B532" s="4"/>
     </row>
-    <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="533" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B533" s="4"/>
     </row>
-    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="534" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B534" s="4"/>
     </row>
-    <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="535" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B535" s="4"/>
     </row>
-    <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="536" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B536" s="4"/>
     </row>
-    <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="537" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B537" s="4"/>
     </row>
-    <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="538" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B538" s="4"/>
     </row>
-    <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="539" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B539" s="4"/>
     </row>
-    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="540" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B540" s="4"/>
     </row>
-    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="541" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B541" s="4"/>
     </row>
-    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="542" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B542" s="4"/>
     </row>
-    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="543" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B543" s="4"/>
     </row>
-    <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="544" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B544" s="4"/>
     </row>
-    <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="545" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B545" s="4"/>
     </row>
-    <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="546" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B546" s="4"/>
     </row>
-    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="547" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B547" s="4"/>
     </row>
-    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="548" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B548" s="4"/>
     </row>
-    <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="549" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B549" s="4"/>
     </row>
-    <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="550" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B550" s="4"/>
     </row>
-    <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="551" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B551" s="4"/>
     </row>
-    <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="552" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B552" s="4"/>
     </row>
-    <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="553" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B553" s="4"/>
     </row>
-    <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="554" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B554" s="4"/>
     </row>
-    <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="555" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B555" s="4"/>
     </row>
-    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="556" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B556" s="4"/>
     </row>
-    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="557" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B557" s="4"/>
     </row>
-    <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="558" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B558" s="4"/>
     </row>
-    <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="559" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B559" s="4"/>
     </row>
-    <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="560" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B560" s="4"/>
     </row>
-    <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="561" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B561" s="4"/>
     </row>
-    <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="562" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B562" s="4"/>
     </row>
-    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="563" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B563" s="4"/>
     </row>
-    <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="564" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B564" s="4"/>
     </row>
-    <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="565" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B565" s="4"/>
     </row>
-    <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="566" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B566" s="4"/>
     </row>
-    <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="567" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B567" s="4"/>
     </row>
-    <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="568" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B568" s="4"/>
     </row>
-    <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="569" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B569" s="4"/>
     </row>
-    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="570" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B570" s="4"/>
     </row>
-    <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="571" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B571" s="4"/>
     </row>
-    <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="572" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B572" s="4"/>
     </row>
-    <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="573" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B573" s="4"/>
     </row>
-    <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="574" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B574" s="4"/>
     </row>
-    <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="575" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B575" s="4"/>
     </row>
-    <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="576" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B576" s="4"/>
     </row>
-    <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="577" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B577" s="4"/>
     </row>
-    <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="578" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B578" s="4"/>
     </row>
-    <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="579" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B579" s="4"/>
     </row>
-    <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="580" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B580" s="4"/>
     </row>
-    <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="581" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B581" s="4"/>
     </row>
-    <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="582" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B582" s="4"/>
     </row>
-    <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="583" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B583" s="4"/>
     </row>
-    <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="584" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B584" s="4"/>
     </row>
-    <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="585" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B585" s="4"/>
     </row>
-    <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="586" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B586" s="4"/>
     </row>
-    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="587" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B587" s="4"/>
     </row>
-    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="588" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B588" s="4"/>
     </row>
-    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="589" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B589" s="4"/>
     </row>
-    <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="590" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B590" s="4"/>
     </row>
-    <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="591" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B591" s="4"/>
     </row>
-    <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="592" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B592" s="4"/>
     </row>
-    <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="593" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B593" s="4"/>
     </row>
-    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="594" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B594" s="4"/>
     </row>
-    <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="595" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B595" s="4"/>
     </row>
-    <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="596" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B596" s="4"/>
     </row>
-    <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="597" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B597" s="4"/>
     </row>
-    <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="598" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B598" s="4"/>
     </row>
-    <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="599" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B599" s="4"/>
     </row>
-    <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="600" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B600" s="4"/>
     </row>
-    <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="601" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B601" s="4"/>
     </row>
-    <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="602" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B602" s="4"/>
     </row>
-    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="603" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B603" s="4"/>
     </row>
-    <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="604" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B604" s="4"/>
     </row>
-    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="605" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B605" s="4"/>
     </row>
-    <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="606" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B606" s="4"/>
     </row>
-    <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="607" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B607" s="4"/>
     </row>
-    <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="608" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B608" s="4"/>
     </row>
-    <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="609" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B609" s="4"/>
     </row>
-    <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="610" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B610" s="4"/>
     </row>
-    <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="611" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B611" s="4"/>
     </row>
-    <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="612" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B612" s="4"/>
     </row>
-    <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="613" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B613" s="4"/>
     </row>
-    <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="614" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B614" s="4"/>
     </row>
-    <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="615" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B615" s="4"/>
     </row>
-    <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="616" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B616" s="4"/>
     </row>
-    <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="617" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B617" s="4"/>
     </row>
-    <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="618" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B618" s="4"/>
     </row>
-    <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="619" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B619" s="4"/>
     </row>
-    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="620" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B620" s="4"/>
     </row>
-    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="621" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B621" s="4"/>
     </row>
-    <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="622" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B622" s="4"/>
     </row>
-    <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="623" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B623" s="4"/>
     </row>
-    <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="624" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B624" s="4"/>
     </row>
-    <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="625" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B625" s="4"/>
     </row>
-    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="626" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B626" s="4"/>
     </row>
-    <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="627" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B627" s="4"/>
     </row>
-    <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="628" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B628" s="4"/>
     </row>
-    <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="629" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B629" s="4"/>
     </row>
-    <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="630" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B630" s="4"/>
     </row>
-    <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="631" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B631" s="4"/>
     </row>
-    <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="632" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B632" s="4"/>
     </row>
-    <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="633" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B633" s="4"/>
     </row>
-    <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="634" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B634" s="4"/>
     </row>
-    <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="635" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B635" s="4"/>
     </row>
-    <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="636" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B636" s="4"/>
     </row>
-    <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="637" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B637" s="4"/>
     </row>
-    <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="638" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B638" s="4"/>
     </row>
-    <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="639" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B639" s="4"/>
     </row>
-    <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="640" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B640" s="4"/>
     </row>
-    <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="641" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B641" s="4"/>
     </row>
-    <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="642" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B642" s="4"/>
     </row>
-    <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="643" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B643" s="4"/>
     </row>
-    <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="644" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B644" s="4"/>
     </row>
-    <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="645" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B645" s="4"/>
     </row>
-    <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="646" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B646" s="4"/>
     </row>
-    <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="647" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B647" s="4"/>
     </row>
-    <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="648" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B648" s="4"/>
     </row>
-    <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="649" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B649" s="4"/>
     </row>
-    <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="650" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B650" s="4"/>
     </row>
-    <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="651" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B651" s="4"/>
     </row>
-    <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="652" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B652" s="4"/>
     </row>
-    <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="653" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B653" s="4"/>
     </row>
-    <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="654" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B654" s="4"/>
     </row>
-    <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="655" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B655" s="4"/>
     </row>
-    <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="656" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B656" s="4"/>
     </row>
-    <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="657" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B657" s="4"/>
     </row>
-    <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="658" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B658" s="4"/>
     </row>
-    <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="659" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B659" s="4"/>
     </row>
-    <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="660" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B660" s="4"/>
     </row>
-    <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="661" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B661" s="4"/>
     </row>
-    <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="662" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B662" s="4"/>
     </row>
-    <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="663" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B663" s="4"/>
     </row>
-    <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="664" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B664" s="4"/>
     </row>
-    <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="665" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B665" s="4"/>
     </row>
-    <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="666" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B666" s="4"/>
     </row>
-    <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="667" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B667" s="4"/>
     </row>
-    <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="668" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B668" s="4"/>
     </row>
-    <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="669" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B669" s="4"/>
     </row>
-    <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="670" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B670" s="4"/>
     </row>
-    <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="671" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B671" s="4"/>
     </row>
-    <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="672" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B672" s="4"/>
     </row>
-    <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="673" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B673" s="4"/>
     </row>
-    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="674" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B674" s="4"/>
     </row>
-    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="675" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B675" s="4"/>
     </row>
-    <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="676" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B676" s="4"/>
     </row>
-    <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="677" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B677" s="4"/>
     </row>
-    <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="678" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B678" s="4"/>
     </row>
-    <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="679" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B679" s="4"/>
     </row>
-    <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="680" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B680" s="4"/>
     </row>
-    <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="681" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B681" s="4"/>
     </row>
-    <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="682" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B682" s="4"/>
     </row>
-    <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="683" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B683" s="4"/>
     </row>
-    <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="684" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B684" s="4"/>
     </row>
-    <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="685" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B685" s="4"/>
     </row>
-    <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="686" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B686" s="4"/>
     </row>
-    <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="687" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B687" s="4"/>
     </row>
-    <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="688" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B688" s="4"/>
     </row>
-    <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="689" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B689" s="4"/>
     </row>
-    <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="690" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B690" s="4"/>
     </row>
-    <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="691" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B691" s="4"/>
     </row>
-    <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="692" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B692" s="4"/>
     </row>
-    <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="693" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B693" s="4"/>
     </row>
-    <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="694" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B694" s="4"/>
     </row>
-    <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="695" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B695" s="4"/>
     </row>
-    <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="696" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B696" s="4"/>
     </row>
-    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="697" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B697" s="4"/>
     </row>
-    <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="698" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B698" s="4"/>
     </row>
-    <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="699" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B699" s="4"/>
     </row>
-    <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="700" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B700" s="4"/>
     </row>
-    <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="701" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B701" s="4"/>
     </row>
-    <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="702" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B702" s="4"/>
     </row>
-    <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="703" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B703" s="4"/>
     </row>
-    <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="704" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B704" s="4"/>
     </row>
-    <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="705" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B705" s="4"/>
     </row>
-    <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="706" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B706" s="4"/>
     </row>
-    <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="707" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B707" s="4"/>
     </row>
-    <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="708" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B708" s="4"/>
     </row>
-    <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="709" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B709" s="4"/>
     </row>
-    <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="710" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B710" s="4"/>
     </row>
-    <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="711" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B711" s="4"/>
     </row>
-    <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="712" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B712" s="4"/>
     </row>
-    <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="713" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B713" s="4"/>
     </row>
-    <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="714" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B714" s="4"/>
     </row>
-    <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="715" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B715" s="4"/>
     </row>
-    <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="716" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B716" s="4"/>
     </row>
-    <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="717" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B717" s="4"/>
     </row>
-    <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="718" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B718" s="4"/>
     </row>
-    <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="719" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B719" s="4"/>
     </row>
-    <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="720" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B720" s="4"/>
     </row>
-    <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="721" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B721" s="4"/>
     </row>
-    <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="722" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B722" s="4"/>
     </row>
-    <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="723" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B723" s="4"/>
     </row>
-    <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="724" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B724" s="4"/>
     </row>
-    <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="725" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B725" s="4"/>
     </row>
-    <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="726" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B726" s="4"/>
     </row>
-    <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="727" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B727" s="4"/>
     </row>
-    <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="728" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B728" s="4"/>
     </row>
-    <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="729" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B729" s="4"/>
     </row>
-    <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="730" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B730" s="4"/>
     </row>
-    <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="731" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B731" s="4"/>
     </row>
-    <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="732" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B732" s="4"/>
     </row>
-    <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="733" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B733" s="4"/>
     </row>
-    <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="734" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B734" s="4"/>
     </row>
-    <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="735" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B735" s="4"/>
     </row>
-    <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="736" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B736" s="4"/>
     </row>
-    <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="737" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B737" s="4"/>
     </row>
-    <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="738" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B738" s="4"/>
     </row>
-    <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="739" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B739" s="4"/>
     </row>
-    <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="740" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B740" s="4"/>
     </row>
-    <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="741" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B741" s="4"/>
     </row>
-    <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="742" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B742" s="4"/>
     </row>
-    <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="743" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B743" s="4"/>
     </row>
-    <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="744" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B744" s="4"/>
     </row>
-    <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="745" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B745" s="4"/>
     </row>
-    <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="746" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B746" s="4"/>
     </row>
-    <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="747" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B747" s="4"/>
     </row>
-    <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="748" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B748" s="4"/>
     </row>
-    <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="749" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B749" s="4"/>
     </row>
-    <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="750" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B750" s="4"/>
     </row>
-    <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="751" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B751" s="4"/>
     </row>
-    <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="752" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B752" s="4"/>
     </row>
-    <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="753" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B753" s="4"/>
     </row>
-    <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="754" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B754" s="4"/>
     </row>
-    <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="755" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B755" s="4"/>
     </row>
-    <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="756" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B756" s="4"/>
     </row>
-    <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="757" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B757" s="4"/>
     </row>
-    <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="758" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B758" s="4"/>
     </row>
-    <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="759" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B759" s="4"/>
     </row>
-    <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="760" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B760" s="4"/>
     </row>
-    <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="761" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B761" s="4"/>
     </row>
-    <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="762" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B762" s="4"/>
     </row>
-    <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="763" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B763" s="4"/>
     </row>
-    <row r="764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="764" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B764" s="4"/>
     </row>
-    <row r="765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="765" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B765" s="4"/>
     </row>
-    <row r="766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="766" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B766" s="4"/>
     </row>
-    <row r="767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="767" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B767" s="4"/>
     </row>
-    <row r="768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="768" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B768" s="4"/>
     </row>
-    <row r="769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="769" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B769" s="4"/>
     </row>
-    <row r="770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="770" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B770" s="4"/>
     </row>
-    <row r="771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="771" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B771" s="4"/>
     </row>
-    <row r="772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="772" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B772" s="4"/>
     </row>
-    <row r="773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="773" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B773" s="4"/>
     </row>
-    <row r="774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="774" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B774" s="4"/>
     </row>
-    <row r="775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="775" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B775" s="4"/>
     </row>
-    <row r="776" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="776" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B776" s="4"/>
     </row>
-    <row r="777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="777" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B777" s="4"/>
     </row>
-    <row r="778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="778" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B778" s="4"/>
     </row>
-    <row r="779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="779" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B779" s="4"/>
     </row>
-    <row r="780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="780" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B780" s="4"/>
     </row>
-    <row r="781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="781" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B781" s="4"/>
     </row>
-    <row r="782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="782" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B782" s="4"/>
     </row>
-    <row r="783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="783" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B783" s="4"/>
     </row>
-    <row r="784" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="784" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B784" s="4"/>
     </row>
-    <row r="785" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="785" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B785" s="4"/>
     </row>
-    <row r="786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="786" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B786" s="4"/>
     </row>
-    <row r="787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="787" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B787" s="4"/>
     </row>
-    <row r="788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="788" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B788" s="4"/>
     </row>
-    <row r="789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="789" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B789" s="4"/>
     </row>
-    <row r="790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="790" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B790" s="4"/>
     </row>
-    <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="791" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B791" s="4"/>
     </row>
-    <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="792" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B792" s="4"/>
     </row>
-    <row r="793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="793" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B793" s="4"/>
     </row>
-    <row r="794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="794" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B794" s="4"/>
     </row>
-    <row r="795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="795" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B795" s="4"/>
     </row>
-    <row r="796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="796" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B796" s="4"/>
     </row>
-    <row r="797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="797" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B797" s="4"/>
     </row>
-    <row r="798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="798" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B798" s="4"/>
     </row>
-    <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="799" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B799" s="4"/>
     </row>
-    <row r="800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="800" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B800" s="4"/>
     </row>
-    <row r="801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="801" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B801" s="4"/>
     </row>
-    <row r="802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="802" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B802" s="4"/>
     </row>
-    <row r="803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="803" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B803" s="4"/>
     </row>
-    <row r="804" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="804" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B804" s="4"/>
     </row>
-    <row r="805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="805" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B805" s="4"/>
     </row>
-    <row r="806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="806" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B806" s="4"/>
     </row>
-    <row r="807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="807" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B807" s="4"/>
     </row>
-    <row r="808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="808" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B808" s="4"/>
     </row>
-    <row r="809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="809" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B809" s="4"/>
     </row>
-    <row r="810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="810" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B810" s="4"/>
     </row>
-    <row r="811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="811" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B811" s="4"/>
     </row>
-    <row r="812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="812" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B812" s="4"/>
     </row>
-    <row r="813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="813" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B813" s="4"/>
     </row>
-    <row r="814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="814" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B814" s="4"/>
     </row>
-    <row r="815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="815" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B815" s="4"/>
     </row>
-    <row r="816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="816" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B816" s="4"/>
     </row>
-    <row r="817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="817" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B817" s="4"/>
     </row>
-    <row r="818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="818" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B818" s="4"/>
     </row>
-    <row r="819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="819" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B819" s="4"/>
     </row>
-    <row r="820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="820" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B820" s="4"/>
     </row>
-    <row r="821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="821" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B821" s="4"/>
     </row>
-    <row r="822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="822" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B822" s="4"/>
     </row>
-    <row r="823" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="823" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B823" s="4"/>
     </row>
-    <row r="824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="824" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B824" s="4"/>
     </row>
-    <row r="825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="825" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B825" s="4"/>
     </row>
-    <row r="826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="826" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B826" s="4"/>
     </row>
-    <row r="827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="827" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B827" s="4"/>
     </row>
-    <row r="828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="828" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B828" s="4"/>
     </row>
-    <row r="829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="829" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B829" s="4"/>
     </row>
-    <row r="830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="830" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B830" s="4"/>
     </row>
-    <row r="831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="831" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B831" s="4"/>
     </row>
-    <row r="832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="832" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B832" s="4"/>
     </row>
-    <row r="833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="833" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B833" s="4"/>
     </row>
-    <row r="834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="834" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B834" s="4"/>
     </row>
-    <row r="835" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="835" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B835" s="4"/>
     </row>
-    <row r="836" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="836" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B836" s="4"/>
     </row>
-    <row r="837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="837" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B837" s="4"/>
     </row>
-    <row r="838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="838" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B838" s="4"/>
     </row>
-    <row r="839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="839" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B839" s="4"/>
     </row>
-    <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="840" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B840" s="4"/>
     </row>
-    <row r="841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="841" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B841" s="4"/>
     </row>
-    <row r="842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="842" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B842" s="4"/>
     </row>
-    <row r="843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="843" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B843" s="4"/>
     </row>
-    <row r="844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="844" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B844" s="4"/>
     </row>
-    <row r="845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="845" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B845" s="4"/>
     </row>
-    <row r="846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="846" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B846" s="4"/>
     </row>
-    <row r="847" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="847" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B847" s="4"/>
     </row>
-    <row r="848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="848" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B848" s="4"/>
     </row>
-    <row r="849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="849" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B849" s="4"/>
     </row>
-    <row r="850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="850" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B850" s="4"/>
     </row>
-    <row r="851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="851" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B851" s="4"/>
     </row>
-    <row r="852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="852" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B852" s="4"/>
     </row>
-    <row r="853" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="853" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B853" s="4"/>
     </row>
-    <row r="854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="854" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B854" s="4"/>
     </row>
-    <row r="855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="855" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B855" s="4"/>
     </row>
-    <row r="856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="856" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B856" s="4"/>
     </row>
-    <row r="857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="857" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B857" s="4"/>
     </row>
-    <row r="858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="858" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B858" s="4"/>
     </row>
-    <row r="859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="859" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B859" s="4"/>
     </row>
-    <row r="860" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="860" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B860" s="4"/>
     </row>
-    <row r="861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="861" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B861" s="4"/>
     </row>
-    <row r="862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="862" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B862" s="4"/>
     </row>
-    <row r="863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="863" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B863" s="4"/>
     </row>
-    <row r="864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="864" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B864" s="4"/>
     </row>
-    <row r="865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="865" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B865" s="4"/>
     </row>
-    <row r="866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="866" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B866" s="4"/>
     </row>
-    <row r="867" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="867" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B867" s="4"/>
     </row>
-    <row r="868" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="868" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B868" s="4"/>
     </row>
-    <row r="869" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="869" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B869" s="4"/>
     </row>
-    <row r="870" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="870" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B870" s="4"/>
     </row>
-    <row r="871" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="871" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B871" s="4"/>
     </row>
-    <row r="872" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="872" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B872" s="4"/>
     </row>
-    <row r="873" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="873" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B873" s="4"/>
     </row>
-    <row r="874" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="874" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B874" s="4"/>
     </row>
-    <row r="875" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="875" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B875" s="4"/>
     </row>
-    <row r="876" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="876" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B876" s="4"/>
     </row>
-    <row r="877" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="877" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B877" s="4"/>
     </row>
-    <row r="878" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="878" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B878" s="4"/>
     </row>
-    <row r="879" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="879" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B879" s="4"/>
     </row>
-    <row r="880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="880" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B880" s="4"/>
     </row>
-    <row r="881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="881" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B881" s="4"/>
     </row>
-    <row r="882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="882" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B882" s="4"/>
     </row>
-    <row r="883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="883" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B883" s="4"/>
     </row>
-    <row r="884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="884" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B884" s="4"/>
     </row>
-    <row r="885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="885" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B885" s="4"/>
     </row>
-    <row r="886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="886" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B886" s="4"/>
     </row>
-    <row r="887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="887" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B887" s="4"/>
     </row>
-    <row r="888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="888" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B888" s="4"/>
     </row>
-    <row r="889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="889" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B889" s="4"/>
     </row>
-    <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="890" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B890" s="4"/>
     </row>
-    <row r="891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="891" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B891" s="4"/>
     </row>
-    <row r="892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="892" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B892" s="4"/>
     </row>
-    <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="893" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B893" s="4"/>
     </row>
-    <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="894" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B894" s="4"/>
     </row>
-    <row r="895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="895" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B895" s="4"/>
     </row>
-    <row r="896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="896" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B896" s="4"/>
     </row>
-    <row r="897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="897" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B897" s="4"/>
     </row>
-    <row r="898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="898" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B898" s="4"/>
     </row>
-    <row r="899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="899" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B899" s="4"/>
     </row>
-    <row r="900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="900" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B900" s="4"/>
     </row>
-    <row r="901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="901" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B901" s="4"/>
     </row>
-    <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="902" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B902" s="4"/>
     </row>
-    <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="903" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B903" s="4"/>
     </row>
-    <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="904" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B904" s="4"/>
     </row>
-    <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="905" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B905" s="4"/>
     </row>
-    <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="906" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B906" s="4"/>
     </row>
-    <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="907" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B907" s="4"/>
     </row>
-    <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="908" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B908" s="4"/>
     </row>
-    <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="909" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B909" s="4"/>
     </row>
-    <row r="910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="910" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B910" s="4"/>
     </row>
-    <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="911" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B911" s="4"/>
     </row>
-    <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="912" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B912" s="4"/>
     </row>
-    <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="913" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B913" s="4"/>
     </row>
-    <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="914" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B914" s="4"/>
     </row>
-    <row r="915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="915" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B915" s="4"/>
     </row>
-    <row r="916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="916" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B916" s="4"/>
     </row>
-    <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="917" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B917" s="4"/>
     </row>
-    <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="918" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B918" s="4"/>
     </row>
-    <row r="919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="919" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B919" s="4"/>
     </row>
-    <row r="920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="920" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B920" s="4"/>
     </row>
-    <row r="921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="921" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B921" s="4"/>
     </row>
-    <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="922" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B922" s="4"/>
     </row>
-    <row r="923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="923" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B923" s="4"/>
     </row>
-    <row r="924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="924" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B924" s="4"/>
     </row>
-    <row r="925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="925" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B925" s="4"/>
     </row>
-    <row r="926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="926" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B926" s="4"/>
     </row>
-    <row r="927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="927" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B927" s="4"/>
     </row>
-    <row r="928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="928" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B928" s="4"/>
     </row>
-    <row r="929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="929" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B929" s="4"/>
     </row>
-    <row r="930" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="930" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B930" s="4"/>
     </row>
-    <row r="931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="931" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B931" s="4"/>
     </row>
-    <row r="932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="932" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B932" s="4"/>
     </row>
-    <row r="933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="933" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B933" s="4"/>
     </row>
-    <row r="934" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="934" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B934" s="4"/>
     </row>
-    <row r="935" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="935" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B935" s="4"/>
     </row>
-    <row r="936" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="936" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B936" s="4"/>
     </row>
-    <row r="937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="937" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B937" s="4"/>
     </row>
-    <row r="938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="938" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B938" s="4"/>
     </row>
-    <row r="939" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="939" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B939" s="4"/>
     </row>
-    <row r="940" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="940" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B940" s="4"/>
     </row>
-    <row r="941" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="941" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B941" s="4"/>
     </row>
-    <row r="942" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="942" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B942" s="4"/>
     </row>
-    <row r="943" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="943" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B943" s="4"/>
     </row>
-    <row r="944" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="944" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B944" s="4"/>
     </row>
-    <row r="945" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="945" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B945" s="4"/>
     </row>
-    <row r="946" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="946" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B946" s="4"/>
     </row>
-    <row r="947" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="947" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B947" s="4"/>
     </row>
-    <row r="948" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="948" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B948" s="4"/>
     </row>
-    <row r="949" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="949" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B949" s="4"/>
     </row>
-    <row r="950" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="950" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B950" s="4"/>
     </row>
-    <row r="951" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="951" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B951" s="4"/>
     </row>
-    <row r="952" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="952" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B952" s="4"/>
     </row>
-    <row r="953" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="953" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B953" s="4"/>
     </row>
-    <row r="954" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="954" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B954" s="4"/>
     </row>
-    <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="955" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B955" s="4"/>
     </row>
-    <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="956" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B956" s="4"/>
     </row>
-    <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="957" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B957" s="4"/>
     </row>
-    <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="958" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B958" s="4"/>
     </row>
-    <row r="959" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="959" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B959" s="4"/>
     </row>
-    <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="960" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B960" s="4"/>
     </row>
-    <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="961" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B961" s="4"/>
     </row>
-    <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="962" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B962" s="4"/>
     </row>
-    <row r="963" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="963" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B963" s="4"/>
     </row>
-    <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="964" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B964" s="4"/>
     </row>
-    <row r="965" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="965" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B965" s="4"/>
     </row>
-    <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="966" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B966" s="4"/>
     </row>
-    <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="967" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B967" s="4"/>
     </row>
-    <row r="968" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="968" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B968" s="4"/>
     </row>
-    <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="969" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B969" s="4"/>
     </row>
-    <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="970" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B970" s="4"/>
     </row>
-    <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="971" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B971" s="4"/>
     </row>
-    <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="972" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B972" s="4"/>
     </row>
-    <row r="973" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="973" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B973" s="4"/>
     </row>
-    <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="974" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B974" s="4"/>
     </row>
-    <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="975" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B975" s="4"/>
     </row>
-    <row r="976" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="976" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B976" s="4"/>
     </row>
-    <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="977" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B977" s="4"/>
     </row>
-    <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="978" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B978" s="4"/>
     </row>
-    <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="979" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B979" s="4"/>
     </row>
-    <row r="980" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="980" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B980" s="4"/>
     </row>
-    <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="981" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B981" s="4"/>
     </row>
-    <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="982" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B982" s="4"/>
     </row>
-    <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="983" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B983" s="4"/>
     </row>
-    <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="984" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B984" s="4"/>
     </row>
-    <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="985" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B985" s="4"/>
     </row>
-    <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="986" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B986" s="4"/>
     </row>
-    <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="987" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B987" s="4"/>
     </row>
-    <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="988" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B988" s="4"/>
     </row>
-    <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="989" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B989" s="4"/>
     </row>
-    <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="990" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B990" s="4"/>
     </row>
-    <row r="991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="991" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B991" s="4"/>
     </row>
-    <row r="992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="992" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B992" s="4"/>
     </row>
-    <row r="993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="993" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B993" s="4"/>
     </row>
-    <row r="994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="994" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B994" s="4"/>
     </row>
-    <row r="995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="995" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B995" s="4"/>
     </row>
-    <row r="996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="996" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B996" s="4"/>
     </row>
-    <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="997" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B997" s="4"/>
     </row>
+    <row r="998" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B998" s="4"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>

</xml_diff>